<commit_message>
example with larger nr trials
</commit_message>
<xml_diff>
--- a/stream.xlsx
+++ b/stream.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Coincidences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9936F34F-1F16-4A77-8DA2-A3CCE12F82E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F7582849-8E68-49BB-9795-BCC5D6680550}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020"/>
   </bookViews>
@@ -954,184 +954,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>57</c:v>
+                  <c:v>465</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>299</c:v>
+                  <c:v>3005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>460</c:v>
+                  <c:v>4936</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>598</c:v>
+                  <c:v>6192</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>685</c:v>
+                  <c:v>6987</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>703</c:v>
+                  <c:v>7343</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>764</c:v>
+                  <c:v>7460</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>784</c:v>
+                  <c:v>7381</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>753</c:v>
+                  <c:v>7263</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>665</c:v>
+                  <c:v>6869</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>640</c:v>
+                  <c:v>6561</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>585</c:v>
+                  <c:v>6058</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>598</c:v>
+                  <c:v>5793</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>517</c:v>
+                  <c:v>5330</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>460</c:v>
+                  <c:v>4733</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>461</c:v>
+                  <c:v>4303</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>403</c:v>
+                  <c:v>3952</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>382</c:v>
+                  <c:v>3555</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>317</c:v>
+                  <c:v>3193</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>270</c:v>
+                  <c:v>2965</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>278</c:v>
+                  <c:v>2648</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>225</c:v>
+                  <c:v>2391</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>193</c:v>
+                  <c:v>2052</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>205</c:v>
+                  <c:v>1874</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>141</c:v>
+                  <c:v>1568</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>124</c:v>
+                  <c:v>1485</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>115</c:v>
+                  <c:v>1327</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>114</c:v>
+                  <c:v>1133</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>109</c:v>
+                  <c:v>980</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>88</c:v>
+                  <c:v>883</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>92</c:v>
+                  <c:v>749</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>73</c:v>
+                  <c:v>676</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>69</c:v>
+                  <c:v>587</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>54</c:v>
+                  <c:v>514</c:v>
                 </c:pt>
                 <c:pt idx="34">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>298</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="51">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="35">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="52">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="53">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="37">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="54">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="55">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="39">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="56">
-                  <c:v>0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1365,184 +1365,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>109</c:v>
+                  <c:v>1123</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>185</c:v>
+                  <c:v>1984</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>273</c:v>
+                  <c:v>2673</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>298</c:v>
+                  <c:v>3167</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>337</c:v>
+                  <c:v>3620</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>420</c:v>
+                  <c:v>3834</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>401</c:v>
+                  <c:v>3841</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>447</c:v>
+                  <c:v>4005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>460</c:v>
+                  <c:v>4081</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>411</c:v>
+                  <c:v>4032</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>409</c:v>
+                  <c:v>3965</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>370</c:v>
+                  <c:v>3833</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>380</c:v>
+                  <c:v>3803</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>388</c:v>
+                  <c:v>3720</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>327</c:v>
+                  <c:v>3479</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>352</c:v>
+                  <c:v>3359</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>333</c:v>
+                  <c:v>3277</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>285</c:v>
+                  <c:v>2943</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>272</c:v>
+                  <c:v>2835</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>266</c:v>
+                  <c:v>2649</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>259</c:v>
+                  <c:v>2464</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>254</c:v>
+                  <c:v>2362</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>215</c:v>
+                  <c:v>2228</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>202</c:v>
+                  <c:v>2051</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>187</c:v>
+                  <c:v>1855</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>156</c:v>
+                  <c:v>1766</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>171</c:v>
+                  <c:v>1638</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>163</c:v>
+                  <c:v>1579</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>115</c:v>
+                  <c:v>1407</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>150</c:v>
+                  <c:v>1305</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>117</c:v>
+                  <c:v>1205</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>109</c:v>
+                  <c:v>1165</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>98</c:v>
+                  <c:v>1038</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>99</c:v>
+                  <c:v>966</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>86</c:v>
+                  <c:v>850</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>92</c:v>
+                  <c:v>838</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>83</c:v>
+                  <c:v>774</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>71</c:v>
+                  <c:v>683</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>75</c:v>
+                  <c:v>697</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>59</c:v>
+                  <c:v>572</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>58</c:v>
+                  <c:v>556</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>54</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>32</c:v>
+                  <c:v>406</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>35</c:v>
+                  <c:v>439</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>46</c:v>
+                  <c:v>395</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>32</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>33</c:v>
+                  <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>36</c:v>
+                  <c:v>301</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>35</c:v>
+                  <c:v>238</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>22</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>30</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>14</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>9</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>21</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>13</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>19</c:v>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>17</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>18</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>10</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1776,184 +1776,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65</c:v>
+                  <c:v>474</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>56</c:v>
+                  <c:v>546</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>637</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59</c:v>
+                  <c:v>682</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>772</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>773</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>804</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>837</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>891</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>828</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>863</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>796</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>824</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>718</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>761</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>674</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>628</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>604</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>563</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>391</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>343</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="59">
                   <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2187,184 +2187,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29</c:v>
+                  <c:v>259</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22</c:v>
+                  <c:v>321</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45</c:v>
+                  <c:v>358</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>382</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45</c:v>
+                  <c:v>473</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>57</c:v>
+                  <c:v>471</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50</c:v>
+                  <c:v>496</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>47</c:v>
+                  <c:v>504</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51</c:v>
+                  <c:v>559</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>60</c:v>
+                  <c:v>603</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>63</c:v>
+                  <c:v>673</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>44</c:v>
+                  <c:v>620</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>71</c:v>
+                  <c:v>673</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>77</c:v>
+                  <c:v>693</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>66</c:v>
+                  <c:v>671</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>80</c:v>
+                  <c:v>729</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>87</c:v>
+                  <c:v>738</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>78</c:v>
+                  <c:v>726</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>61</c:v>
+                  <c:v>771</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>82</c:v>
+                  <c:v>771</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>78</c:v>
+                  <c:v>749</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>65</c:v>
+                  <c:v>808</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>72</c:v>
+                  <c:v>735</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>88</c:v>
+                  <c:v>722</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>62</c:v>
+                  <c:v>771</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>86</c:v>
+                  <c:v>770</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>75</c:v>
+                  <c:v>753</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>66</c:v>
+                  <c:v>785</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>65</c:v>
+                  <c:v>739</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>68</c:v>
+                  <c:v>727</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>63</c:v>
+                  <c:v>747</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>78</c:v>
+                  <c:v>691</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>74</c:v>
+                  <c:v>763</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>67</c:v>
+                  <c:v>742</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>64</c:v>
+                  <c:v>731</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>78</c:v>
+                  <c:v>725</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>66</c:v>
+                  <c:v>709</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>80</c:v>
+                  <c:v>688</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>66</c:v>
+                  <c:v>721</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>76</c:v>
+                  <c:v>691</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>63</c:v>
+                  <c:v>711</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>76</c:v>
+                  <c:v>682</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>65</c:v>
+                  <c:v>611</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>57</c:v>
+                  <c:v>642</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>60</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>64</c:v>
+                  <c:v>683</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>57</c:v>
+                  <c:v>596</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>61</c:v>
+                  <c:v>632</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>63</c:v>
+                  <c:v>625</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>56</c:v>
+                  <c:v>635</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>67</c:v>
+                  <c:v>581</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>66</c:v>
+                  <c:v>527</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>46</c:v>
+                  <c:v>551</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>51</c:v>
+                  <c:v>572</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>58</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>46</c:v>
+                  <c:v>553</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2598,184 +2598,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>382</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>161</c:v>
+                  <c:v>1596</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>231</c:v>
+                  <c:v>2492</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>241</c:v>
+                  <c:v>2863</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>302</c:v>
+                  <c:v>3015</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>284</c:v>
+                  <c:v>2765</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240</c:v>
+                  <c:v>2586</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>248</c:v>
+                  <c:v>2407</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>195</c:v>
+                  <c:v>2013</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>78</c:v>
+                  <c:v>1544</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>105</c:v>
+                  <c:v>1229</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36</c:v>
+                  <c:v>752</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>90</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-4</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-82</c:v>
+                  <c:v>-523</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>-592</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-101</c:v>
+                  <c:v>-904</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-97</c:v>
+                  <c:v>-1158</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-99</c:v>
+                  <c:v>-1139</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-154</c:v>
+                  <c:v>-1360</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-150</c:v>
+                  <c:v>-1413</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-172</c:v>
+                  <c:v>-1442</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-176</c:v>
+                  <c:v>-1709</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-150</c:v>
+                  <c:v>-1729</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-202</c:v>
+                  <c:v>-1817</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-181</c:v>
+                  <c:v>-1753</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-168</c:v>
+                  <c:v>-1737</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-204</c:v>
+                  <c:v>-1757</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-174</c:v>
+                  <c:v>-1839</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-166</c:v>
+                  <c:v>-1774</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-178</c:v>
+                  <c:v>-1747</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-159</c:v>
+                  <c:v>-1709</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-148</c:v>
+                  <c:v>-1708</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-155</c:v>
+                  <c:v>-1654</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-147</c:v>
+                  <c:v>-1595</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-149</c:v>
+                  <c:v>-1425</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-163</c:v>
+                  <c:v>-1589</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-145</c:v>
+                  <c:v>-1522</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-133</c:v>
+                  <c:v>-1470</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-156</c:v>
+                  <c:v>-1454</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-128</c:v>
+                  <c:v>-1304</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-148</c:v>
+                  <c:v>-1331</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-128</c:v>
+                  <c:v>-1295</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-112</c:v>
+                  <c:v>-1154</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-113</c:v>
+                  <c:v>-1262</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-142</c:v>
+                  <c:v>-1158</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-100</c:v>
+                  <c:v>-1026</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-94</c:v>
+                  <c:v>-1073</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-113</c:v>
+                  <c:v>-1034</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-109</c:v>
+                  <c:v>-1038</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-83</c:v>
+                  <c:v>-928</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-99</c:v>
+                  <c:v>-939</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-85</c:v>
+                  <c:v>-903</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-83</c:v>
+                  <c:v>-918</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-96</c:v>
+                  <c:v>-798</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-88</c:v>
+                  <c:v>-757</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-77</c:v>
+                  <c:v>-754</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-70</c:v>
+                  <c:v>-762</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-83</c:v>
+                  <c:v>-754</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-61</c:v>
+                  <c:v>-706</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3311,184 +3311,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>0.78125</c:v>
+                  <c:v>0.6970802919708029</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36842105263157893</c:v>
+                  <c:v>0.36157680108744905</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.33526850507982581</c:v>
+                  <c:v>0.33766937669376695</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25235602094240839</c:v>
+                  <c:v>0.30070370759374015</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.28277153558052437</c:v>
+                  <c:v>0.27511634273200108</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.25311942959001782</c:v>
+                  <c:v>0.23194362889019376</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.18633540372670807</c:v>
+                  <c:v>0.20966434246797469</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.18787878787878787</c:v>
+                  <c:v>0.19481991096721976</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.14874141876430205</c:v>
+                  <c:v>0.16087269239990409</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.2300319488817889E-2</c:v>
+                  <c:v>0.1266196490077087</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.9361702127659579E-2</c:v>
+                  <c:v>0.10333809804086437</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.1746031746031744E-2</c:v>
+                  <c:v>6.6173882435762055E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.1374321880650996E-2</c:v>
+                  <c:v>4.6045503791982668E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-3.8535645472061657E-3</c:v>
+                  <c:v>9.0874668686103752E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-8.1836327345309379E-2</c:v>
+                  <c:v>-5.2357593352687956E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.7527352297592995E-3</c:v>
+                  <c:v>-6.4361817786475317E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.1113561190738699</c:v>
+                  <c:v>-0.10263396911898275</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.11265969802555169</c:v>
+                  <c:v>-0.14005805515239478</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.13506139154160982</c:v>
+                  <c:v>-0.15136212624584719</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.22190201729106629</c:v>
+                  <c:v>-0.18655692729766804</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.21246458923512748</c:v>
+                  <c:v>-0.21061260992696379</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.27652733118971062</c:v>
+                  <c:v>-0.23168380462724936</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.31316725978647686</c:v>
+                  <c:v>-0.29399621537932219</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.26785714285714285</c:v>
+                  <c:v>-0.31568376848639768</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.41735537190082644</c:v>
+                  <c:v>-0.36684837472239046</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.42191142191142189</c:v>
+                  <c:v>-0.37116239678170654</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.42211055276381909</c:v>
+                  <c:v>-0.39558187201093142</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.47222222222222221</c:v>
+                  <c:v>-0.43673875217499381</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.44387755102040816</c:v>
+                  <c:v>-0.48407475651487236</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.4853801169590643</c:v>
+                  <c:v>-0.5011299435028248</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-0.49171270718232046</c:v>
+                  <c:v>-0.53836671802773495</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-0.52131147540983602</c:v>
+                  <c:v>-0.55831427638026787</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-0.5174825174825175</c:v>
+                  <c:v>-0.59264399722414984</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-0.58935361216730042</c:v>
+                  <c:v>-0.6167039522744221</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-0.61506276150627615</c:v>
+                  <c:v>-0.6286953094205755</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.61825726141078841</c:v>
+                  <c:v>-0.62692476902771666</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-0.75115207373271886</c:v>
+                  <c:v>-0.69117007394519359</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.6872037914691943</c:v>
+                  <c:v>-0.71860245514636445</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-0.7189189189189189</c:v>
+                  <c:v>-0.74847250509164964</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-0.72222222222222221</c:v>
+                  <c:v>-0.74948453608247423</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-0.7441860465116279</c:v>
+                  <c:v>-0.74942528735632186</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-0.80434782608695654</c:v>
+                  <c:v>-0.80036079374624169</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-0.82051282051282048</c:v>
+                  <c:v>-0.80384854127870886</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-0.8</c:v>
+                  <c:v>-0.78610354223433243</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-0.87596899224806202</c:v>
+                  <c:v>-0.84021304926764317</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-0.93421052631578949</c:v>
+                  <c:v>-0.84773060029282576</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-0.84745762711864403</c:v>
+                  <c:v>-0.83550488599348538</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-0.79661016949152541</c:v>
+                  <c:v>-0.88898094449047227</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-0.91869918699186992</c:v>
+                  <c:v>-0.88527397260273977</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-0.90082644628099173</c:v>
+                  <c:v>-0.90734265734265729</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-0.93258426966292129</c:v>
+                  <c:v>-0.89748549323017413</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-0.94285714285714284</c:v>
+                  <c:v>-0.91076624636275461</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-0.91397849462365588</c:v>
+                  <c:v>-0.90936555891238668</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-0.95402298850574707</c:v>
+                  <c:v>-0.94444444444444442</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-0.96</c:v>
+                  <c:v>-0.92147806004618937</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-0.97777777777777775</c:v>
+                  <c:v>-0.93572311495673666</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-1</c:v>
+                  <c:v>-0.93086419753086425</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-0.94594594594594594</c:v>
+                  <c:v>-0.94306930693069302</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-0.97647058823529409</c:v>
+                  <c:v>-0.94962216624685136</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-0.93846153846153846</c:v>
+                  <c:v>-0.95405405405405408</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4837,14 +4837,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>111125</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4872,15 +4872,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>50799</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:colOff>12699</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>3174</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5208,7 +5208,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5362,23 +5362,23 @@
         <v>1</v>
       </c>
       <c r="B11">
-        <v>57</v>
+        <v>465</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F11">
-        <v>50</v>
+        <v>382</v>
       </c>
       <c r="G11">
         <f>F11/SUM(B11:E11)</f>
-        <v>0.78125</v>
+        <v>0.6970802919708029</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -5386,23 +5386,23 @@
         <v>21</v>
       </c>
       <c r="B12">
-        <v>299</v>
+        <v>3005</v>
       </c>
       <c r="C12">
-        <v>109</v>
+        <v>1123</v>
       </c>
       <c r="D12">
-        <v>20</v>
+        <v>201</v>
       </c>
       <c r="E12">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="F12">
-        <v>161</v>
+        <v>1596</v>
       </c>
       <c r="G12">
         <f t="shared" ref="G12:G70" si="0">F12/SUM(B12:E12)</f>
-        <v>0.36842105263157893</v>
+        <v>0.36157680108744905</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -5410,23 +5410,23 @@
         <v>41</v>
       </c>
       <c r="B13">
-        <v>460</v>
+        <v>4936</v>
       </c>
       <c r="C13">
-        <v>185</v>
+        <v>1984</v>
       </c>
       <c r="D13">
-        <v>28</v>
+        <v>344</v>
       </c>
       <c r="E13">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="F13">
-        <v>231</v>
+        <v>2492</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>0.33526850507982581</v>
+        <v>0.33766937669376695</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -5434,23 +5434,23 @@
         <v>61</v>
       </c>
       <c r="B14">
-        <v>598</v>
+        <v>6192</v>
       </c>
       <c r="C14">
-        <v>273</v>
+        <v>2673</v>
       </c>
       <c r="D14">
-        <v>65</v>
+        <v>474</v>
       </c>
       <c r="E14">
-        <v>19</v>
+        <v>182</v>
       </c>
       <c r="F14">
-        <v>241</v>
+        <v>2863</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>0.25235602094240839</v>
+        <v>0.30070370759374015</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -5458,23 +5458,23 @@
         <v>81</v>
       </c>
       <c r="B15">
-        <v>685</v>
+        <v>6987</v>
       </c>
       <c r="C15">
-        <v>298</v>
+        <v>3167</v>
       </c>
       <c r="D15">
-        <v>56</v>
+        <v>546</v>
       </c>
       <c r="E15">
-        <v>29</v>
+        <v>259</v>
       </c>
       <c r="F15">
-        <v>302</v>
+        <v>3015</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>0.28277153558052437</v>
+        <v>0.27511634273200108</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -5482,23 +5482,23 @@
         <v>101</v>
       </c>
       <c r="B16">
-        <v>703</v>
+        <v>7343</v>
       </c>
       <c r="C16">
-        <v>337</v>
+        <v>3620</v>
       </c>
       <c r="D16">
-        <v>60</v>
+        <v>637</v>
       </c>
       <c r="E16">
-        <v>22</v>
+        <v>321</v>
       </c>
       <c r="F16">
-        <v>284</v>
+        <v>2765</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>0.25311942959001782</v>
+        <v>0.23194362889019376</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -5506,23 +5506,23 @@
         <v>121</v>
       </c>
       <c r="B17">
-        <v>764</v>
+        <v>7460</v>
       </c>
       <c r="C17">
-        <v>420</v>
+        <v>3834</v>
       </c>
       <c r="D17">
-        <v>59</v>
+        <v>682</v>
       </c>
       <c r="E17">
-        <v>45</v>
+        <v>358</v>
       </c>
       <c r="F17">
-        <v>240</v>
+        <v>2586</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>0.18633540372670807</v>
+        <v>0.20966434246797469</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -5530,23 +5530,23 @@
         <v>141</v>
       </c>
       <c r="B18">
-        <v>784</v>
+        <v>7381</v>
       </c>
       <c r="C18">
-        <v>401</v>
+        <v>3841</v>
       </c>
       <c r="D18">
-        <v>85</v>
+        <v>751</v>
       </c>
       <c r="E18">
-        <v>50</v>
+        <v>382</v>
       </c>
       <c r="F18">
-        <v>248</v>
+        <v>2407</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>0.18787878787878787</v>
+        <v>0.19481991096721976</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -5554,23 +5554,23 @@
         <v>161</v>
       </c>
       <c r="B19">
-        <v>753</v>
+        <v>7263</v>
       </c>
       <c r="C19">
-        <v>447</v>
+        <v>4005</v>
       </c>
       <c r="D19">
-        <v>66</v>
+        <v>772</v>
       </c>
       <c r="E19">
-        <v>45</v>
+        <v>473</v>
       </c>
       <c r="F19">
-        <v>195</v>
+        <v>2013</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>0.14874141876430205</v>
+        <v>0.16087269239990409</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -5578,23 +5578,23 @@
         <v>181</v>
       </c>
       <c r="B20">
-        <v>665</v>
+        <v>6869</v>
       </c>
       <c r="C20">
-        <v>460</v>
+        <v>4081</v>
       </c>
       <c r="D20">
-        <v>70</v>
+        <v>773</v>
       </c>
       <c r="E20">
-        <v>57</v>
+        <v>471</v>
       </c>
       <c r="F20">
-        <v>78</v>
+        <v>1544</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>6.2300319488817889E-2</v>
+        <v>0.1266196490077087</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -5602,23 +5602,23 @@
         <v>201</v>
       </c>
       <c r="B21">
-        <v>640</v>
+        <v>6561</v>
       </c>
       <c r="C21">
-        <v>411</v>
+        <v>4032</v>
       </c>
       <c r="D21">
-        <v>74</v>
+        <v>804</v>
       </c>
       <c r="E21">
-        <v>50</v>
+        <v>496</v>
       </c>
       <c r="F21">
-        <v>105</v>
+        <v>1229</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>8.9361702127659579E-2</v>
+        <v>0.10333809804086437</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -5626,23 +5626,23 @@
         <v>221</v>
       </c>
       <c r="B22">
-        <v>585</v>
+        <v>6058</v>
       </c>
       <c r="C22">
-        <v>409</v>
+        <v>3965</v>
       </c>
       <c r="D22">
-        <v>93</v>
+        <v>837</v>
       </c>
       <c r="E22">
-        <v>47</v>
+        <v>504</v>
       </c>
       <c r="F22">
-        <v>36</v>
+        <v>752</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
-        <v>3.1746031746031744E-2</v>
+        <v>6.6173882435762055E-2</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -5650,23 +5650,23 @@
         <v>241</v>
       </c>
       <c r="B23">
-        <v>598</v>
+        <v>5793</v>
       </c>
       <c r="C23">
-        <v>370</v>
+        <v>3833</v>
       </c>
       <c r="D23">
-        <v>87</v>
+        <v>891</v>
       </c>
       <c r="E23">
-        <v>51</v>
+        <v>559</v>
       </c>
       <c r="F23">
-        <v>90</v>
+        <v>510</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>8.1374321880650996E-2</v>
+        <v>4.6045503791982668E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -5674,23 +5674,23 @@
         <v>261</v>
       </c>
       <c r="B24">
-        <v>517</v>
+        <v>5330</v>
       </c>
       <c r="C24">
-        <v>380</v>
+        <v>3803</v>
       </c>
       <c r="D24">
-        <v>81</v>
+        <v>828</v>
       </c>
       <c r="E24">
-        <v>60</v>
+        <v>603</v>
       </c>
       <c r="F24">
-        <v>-4</v>
+        <v>96</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>-3.8535645472061657E-3</v>
+        <v>9.0874668686103752E-3</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -5698,23 +5698,23 @@
         <v>281</v>
       </c>
       <c r="B25">
-        <v>460</v>
+        <v>4733</v>
       </c>
       <c r="C25">
-        <v>388</v>
+        <v>3720</v>
       </c>
       <c r="D25">
-        <v>91</v>
+        <v>863</v>
       </c>
       <c r="E25">
-        <v>63</v>
+        <v>673</v>
       </c>
       <c r="F25">
-        <v>-82</v>
+        <v>-523</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
-        <v>-8.1836327345309379E-2</v>
+        <v>-5.2357593352687956E-2</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -5722,23 +5722,23 @@
         <v>301</v>
       </c>
       <c r="B26">
-        <v>461</v>
+        <v>4303</v>
       </c>
       <c r="C26">
-        <v>327</v>
+        <v>3479</v>
       </c>
       <c r="D26">
-        <v>82</v>
+        <v>796</v>
       </c>
       <c r="E26">
-        <v>44</v>
+        <v>620</v>
       </c>
       <c r="F26">
-        <v>8</v>
+        <v>-592</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>8.7527352297592995E-3</v>
+        <v>-6.4361817786475317E-2</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -5746,23 +5746,23 @@
         <v>321</v>
       </c>
       <c r="B27">
-        <v>403</v>
+        <v>3952</v>
       </c>
       <c r="C27">
-        <v>352</v>
+        <v>3359</v>
       </c>
       <c r="D27">
-        <v>81</v>
+        <v>824</v>
       </c>
       <c r="E27">
-        <v>71</v>
+        <v>673</v>
       </c>
       <c r="F27">
-        <v>-101</v>
+        <v>-904</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>-0.1113561190738699</v>
+        <v>-0.10263396911898275</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -5770,23 +5770,23 @@
         <v>341</v>
       </c>
       <c r="B28">
-        <v>382</v>
+        <v>3555</v>
       </c>
       <c r="C28">
-        <v>333</v>
+        <v>3277</v>
       </c>
       <c r="D28">
-        <v>69</v>
+        <v>743</v>
       </c>
       <c r="E28">
-        <v>77</v>
+        <v>693</v>
       </c>
       <c r="F28">
-        <v>-97</v>
+        <v>-1158</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
-        <v>-0.11265969802555169</v>
+        <v>-0.14005805515239478</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -5794,23 +5794,23 @@
         <v>361</v>
       </c>
       <c r="B29">
-        <v>317</v>
+        <v>3193</v>
       </c>
       <c r="C29">
-        <v>285</v>
+        <v>2943</v>
       </c>
       <c r="D29">
-        <v>65</v>
+        <v>718</v>
       </c>
       <c r="E29">
-        <v>66</v>
+        <v>671</v>
       </c>
       <c r="F29">
-        <v>-99</v>
+        <v>-1139</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
-        <v>-0.13506139154160982</v>
+        <v>-0.15136212624584719</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -5818,23 +5818,23 @@
         <v>381</v>
       </c>
       <c r="B30">
-        <v>270</v>
+        <v>2965</v>
       </c>
       <c r="C30">
-        <v>272</v>
+        <v>2835</v>
       </c>
       <c r="D30">
-        <v>72</v>
+        <v>761</v>
       </c>
       <c r="E30">
-        <v>80</v>
+        <v>729</v>
       </c>
       <c r="F30">
-        <v>-154</v>
+        <v>-1360</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
-        <v>-0.22190201729106629</v>
+        <v>-0.18655692729766804</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -5842,23 +5842,23 @@
         <v>401</v>
       </c>
       <c r="B31">
-        <v>278</v>
+        <v>2648</v>
       </c>
       <c r="C31">
-        <v>266</v>
+        <v>2649</v>
       </c>
       <c r="D31">
-        <v>75</v>
+        <v>674</v>
       </c>
       <c r="E31">
-        <v>87</v>
+        <v>738</v>
       </c>
       <c r="F31">
-        <v>-150</v>
+        <v>-1413</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
-        <v>-0.21246458923512748</v>
+        <v>-0.21061260992696379</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -5866,23 +5866,23 @@
         <v>421</v>
       </c>
       <c r="B32">
-        <v>225</v>
+        <v>2391</v>
       </c>
       <c r="C32">
-        <v>259</v>
+        <v>2464</v>
       </c>
       <c r="D32">
-        <v>60</v>
+        <v>643</v>
       </c>
       <c r="E32">
-        <v>78</v>
+        <v>726</v>
       </c>
       <c r="F32">
-        <v>-172</v>
+        <v>-1442</v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
-        <v>-0.27652733118971062</v>
+        <v>-0.23168380462724936</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -5890,23 +5890,23 @@
         <v>441</v>
       </c>
       <c r="B33">
-        <v>193</v>
+        <v>2052</v>
       </c>
       <c r="C33">
-        <v>254</v>
+        <v>2362</v>
       </c>
       <c r="D33">
-        <v>54</v>
+        <v>628</v>
       </c>
       <c r="E33">
-        <v>61</v>
+        <v>771</v>
       </c>
       <c r="F33">
-        <v>-176</v>
+        <v>-1709</v>
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
-        <v>-0.31316725978647686</v>
+        <v>-0.29399621537932219</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -5914,23 +5914,23 @@
         <v>461</v>
       </c>
       <c r="B34">
-        <v>205</v>
+        <v>1874</v>
       </c>
       <c r="C34">
-        <v>215</v>
+        <v>2228</v>
       </c>
       <c r="D34">
-        <v>58</v>
+        <v>604</v>
       </c>
       <c r="E34">
-        <v>82</v>
+        <v>771</v>
       </c>
       <c r="F34">
-        <v>-150</v>
+        <v>-1729</v>
       </c>
       <c r="G34">
         <f t="shared" si="0"/>
-        <v>-0.26785714285714285</v>
+        <v>-0.31568376848639768</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -5938,23 +5938,23 @@
         <v>481</v>
       </c>
       <c r="B35">
-        <v>141</v>
+        <v>1568</v>
       </c>
       <c r="C35">
-        <v>202</v>
+        <v>2051</v>
       </c>
       <c r="D35">
-        <v>63</v>
+        <v>585</v>
       </c>
       <c r="E35">
-        <v>78</v>
+        <v>749</v>
       </c>
       <c r="F35">
-        <v>-202</v>
+        <v>-1817</v>
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
-        <v>-0.41735537190082644</v>
+        <v>-0.36684837472239046</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -5962,23 +5962,23 @@
         <v>501</v>
       </c>
       <c r="B36">
-        <v>124</v>
+        <v>1485</v>
       </c>
       <c r="C36">
-        <v>187</v>
+        <v>1855</v>
       </c>
       <c r="D36">
-        <v>53</v>
+        <v>575</v>
       </c>
       <c r="E36">
-        <v>65</v>
+        <v>808</v>
       </c>
       <c r="F36">
-        <v>-181</v>
+        <v>-1753</v>
       </c>
       <c r="G36">
         <f t="shared" si="0"/>
-        <v>-0.42191142191142189</v>
+        <v>-0.37116239678170654</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -5986,23 +5986,23 @@
         <v>521</v>
       </c>
       <c r="B37">
-        <v>115</v>
+        <v>1327</v>
       </c>
       <c r="C37">
-        <v>156</v>
+        <v>1766</v>
       </c>
       <c r="D37">
-        <v>55</v>
+        <v>563</v>
       </c>
       <c r="E37">
-        <v>72</v>
+        <v>735</v>
       </c>
       <c r="F37">
-        <v>-168</v>
+        <v>-1737</v>
       </c>
       <c r="G37">
         <f t="shared" si="0"/>
-        <v>-0.42211055276381909</v>
+        <v>-0.39558187201093142</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -6010,23 +6010,23 @@
         <v>541</v>
       </c>
       <c r="B38">
-        <v>114</v>
+        <v>1133</v>
       </c>
       <c r="C38">
-        <v>171</v>
+        <v>1638</v>
       </c>
       <c r="D38">
-        <v>59</v>
+        <v>530</v>
       </c>
       <c r="E38">
-        <v>88</v>
+        <v>722</v>
       </c>
       <c r="F38">
-        <v>-204</v>
+        <v>-1757</v>
       </c>
       <c r="G38">
         <f t="shared" si="0"/>
-        <v>-0.47222222222222221</v>
+        <v>-0.43673875217499381</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -6034,23 +6034,23 @@
         <v>561</v>
       </c>
       <c r="B39">
-        <v>109</v>
+        <v>980</v>
       </c>
       <c r="C39">
-        <v>163</v>
+        <v>1579</v>
       </c>
       <c r="D39">
-        <v>58</v>
+        <v>469</v>
       </c>
       <c r="E39">
-        <v>62</v>
+        <v>771</v>
       </c>
       <c r="F39">
-        <v>-174</v>
+        <v>-1839</v>
       </c>
       <c r="G39">
         <f t="shared" si="0"/>
-        <v>-0.44387755102040816</v>
+        <v>-0.48407475651487236</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -6058,23 +6058,23 @@
         <v>581</v>
       </c>
       <c r="B40">
-        <v>88</v>
+        <v>883</v>
       </c>
       <c r="C40">
-        <v>115</v>
+        <v>1407</v>
       </c>
       <c r="D40">
-        <v>53</v>
+        <v>480</v>
       </c>
       <c r="E40">
-        <v>86</v>
+        <v>770</v>
       </c>
       <c r="F40">
-        <v>-166</v>
+        <v>-1774</v>
       </c>
       <c r="G40">
         <f t="shared" si="0"/>
-        <v>-0.4853801169590643</v>
+        <v>-0.5011299435028248</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -6082,23 +6082,23 @@
         <v>601</v>
       </c>
       <c r="B41">
-        <v>92</v>
+        <v>749</v>
       </c>
       <c r="C41">
-        <v>150</v>
+        <v>1305</v>
       </c>
       <c r="D41">
-        <v>45</v>
+        <v>438</v>
       </c>
       <c r="E41">
-        <v>75</v>
+        <v>753</v>
       </c>
       <c r="F41">
-        <v>-178</v>
+        <v>-1747</v>
       </c>
       <c r="G41">
         <f t="shared" si="0"/>
-        <v>-0.49171270718232046</v>
+        <v>-0.53836671802773495</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -6106,23 +6106,23 @@
         <v>621</v>
       </c>
       <c r="B42">
-        <v>73</v>
+        <v>676</v>
       </c>
       <c r="C42">
-        <v>117</v>
+        <v>1205</v>
       </c>
       <c r="D42">
-        <v>49</v>
+        <v>395</v>
       </c>
       <c r="E42">
-        <v>66</v>
+        <v>785</v>
       </c>
       <c r="F42">
-        <v>-159</v>
+        <v>-1709</v>
       </c>
       <c r="G42">
         <f t="shared" si="0"/>
-        <v>-0.52131147540983602</v>
+        <v>-0.55831427638026787</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -6130,23 +6130,23 @@
         <v>641</v>
       </c>
       <c r="B43">
-        <v>69</v>
+        <v>587</v>
       </c>
       <c r="C43">
-        <v>109</v>
+        <v>1165</v>
       </c>
       <c r="D43">
-        <v>43</v>
+        <v>391</v>
       </c>
       <c r="E43">
-        <v>65</v>
+        <v>739</v>
       </c>
       <c r="F43">
-        <v>-148</v>
+        <v>-1708</v>
       </c>
       <c r="G43">
         <f t="shared" si="0"/>
-        <v>-0.5174825174825175</v>
+        <v>-0.59264399722414984</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -6154,23 +6154,23 @@
         <v>661</v>
       </c>
       <c r="B44">
-        <v>54</v>
+        <v>514</v>
       </c>
       <c r="C44">
-        <v>98</v>
+        <v>1038</v>
       </c>
       <c r="D44">
-        <v>43</v>
+        <v>403</v>
       </c>
       <c r="E44">
-        <v>68</v>
+        <v>727</v>
       </c>
       <c r="F44">
-        <v>-155</v>
+        <v>-1654</v>
       </c>
       <c r="G44">
         <f t="shared" si="0"/>
-        <v>-0.58935361216730042</v>
+        <v>-0.6167039522744221</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -6178,23 +6178,23 @@
         <v>681</v>
       </c>
       <c r="B45">
-        <v>46</v>
+        <v>471</v>
       </c>
       <c r="C45">
-        <v>99</v>
+        <v>966</v>
       </c>
       <c r="D45">
-        <v>31</v>
+        <v>353</v>
       </c>
       <c r="E45">
-        <v>63</v>
+        <v>747</v>
       </c>
       <c r="F45">
-        <v>-147</v>
+        <v>-1595</v>
       </c>
       <c r="G45">
         <f t="shared" si="0"/>
-        <v>-0.61506276150627615</v>
+        <v>-0.6286953094205755</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -6202,23 +6202,23 @@
         <v>701</v>
       </c>
       <c r="B46">
-        <v>46</v>
+        <v>424</v>
       </c>
       <c r="C46">
-        <v>86</v>
+        <v>850</v>
       </c>
       <c r="D46">
-        <v>31</v>
+        <v>308</v>
       </c>
       <c r="E46">
-        <v>78</v>
+        <v>691</v>
       </c>
       <c r="F46">
-        <v>-149</v>
+        <v>-1425</v>
       </c>
       <c r="G46">
         <f t="shared" si="0"/>
-        <v>-0.61825726141078841</v>
+        <v>-0.62692476902771666</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -6226,23 +6226,23 @@
         <v>721</v>
       </c>
       <c r="B47">
-        <v>27</v>
+        <v>355</v>
       </c>
       <c r="C47">
-        <v>92</v>
+        <v>838</v>
       </c>
       <c r="D47">
-        <v>24</v>
+        <v>343</v>
       </c>
       <c r="E47">
-        <v>74</v>
+        <v>763</v>
       </c>
       <c r="F47">
-        <v>-163</v>
+        <v>-1589</v>
       </c>
       <c r="G47">
         <f t="shared" si="0"/>
-        <v>-0.75115207373271886</v>
+        <v>-0.69117007394519359</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -6250,23 +6250,23 @@
         <v>741</v>
       </c>
       <c r="B48">
-        <v>33</v>
+        <v>298</v>
       </c>
       <c r="C48">
-        <v>83</v>
+        <v>774</v>
       </c>
       <c r="D48">
-        <v>28</v>
+        <v>304</v>
       </c>
       <c r="E48">
-        <v>67</v>
+        <v>742</v>
       </c>
       <c r="F48">
-        <v>-145</v>
+        <v>-1522</v>
       </c>
       <c r="G48">
         <f t="shared" si="0"/>
-        <v>-0.6872037914691943</v>
+        <v>-0.71860245514636445</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -6274,23 +6274,23 @@
         <v>761</v>
       </c>
       <c r="B49">
-        <v>26</v>
+        <v>247</v>
       </c>
       <c r="C49">
-        <v>71</v>
+        <v>683</v>
       </c>
       <c r="D49">
-        <v>24</v>
+        <v>303</v>
       </c>
       <c r="E49">
-        <v>64</v>
+        <v>731</v>
       </c>
       <c r="F49">
-        <v>-133</v>
+        <v>-1470</v>
       </c>
       <c r="G49">
         <f t="shared" si="0"/>
-        <v>-0.7189189189189189</v>
+        <v>-0.74847250509164964</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
@@ -6298,23 +6298,23 @@
         <v>781</v>
       </c>
       <c r="B50">
-        <v>30</v>
+        <v>243</v>
       </c>
       <c r="C50">
-        <v>75</v>
+        <v>697</v>
       </c>
       <c r="D50">
-        <v>33</v>
+        <v>275</v>
       </c>
       <c r="E50">
-        <v>78</v>
+        <v>725</v>
       </c>
       <c r="F50">
-        <v>-156</v>
+        <v>-1454</v>
       </c>
       <c r="G50">
         <f t="shared" si="0"/>
-        <v>-0.72222222222222221</v>
+        <v>-0.74948453608247423</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -6322,23 +6322,23 @@
         <v>801</v>
       </c>
       <c r="B51">
-        <v>22</v>
+        <v>218</v>
       </c>
       <c r="C51">
-        <v>59</v>
+        <v>572</v>
       </c>
       <c r="D51">
-        <v>25</v>
+        <v>241</v>
       </c>
       <c r="E51">
-        <v>66</v>
+        <v>709</v>
       </c>
       <c r="F51">
-        <v>-128</v>
+        <v>-1304</v>
       </c>
       <c r="G51">
         <f t="shared" si="0"/>
-        <v>-0.7441860465116279</v>
+        <v>-0.74942528735632186</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
@@ -6346,23 +6346,23 @@
         <v>821</v>
       </c>
       <c r="B52">
-        <v>18</v>
+        <v>166</v>
       </c>
       <c r="C52">
-        <v>58</v>
+        <v>556</v>
       </c>
       <c r="D52">
-        <v>28</v>
+        <v>253</v>
       </c>
       <c r="E52">
-        <v>80</v>
+        <v>688</v>
       </c>
       <c r="F52">
-        <v>-148</v>
+        <v>-1331</v>
       </c>
       <c r="G52">
         <f t="shared" si="0"/>
-        <v>-0.80434782608695654</v>
+        <v>-0.80036079374624169</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
@@ -6370,23 +6370,23 @@
         <v>841</v>
       </c>
       <c r="B53">
-        <v>14</v>
+        <v>158</v>
       </c>
       <c r="C53">
-        <v>54</v>
+        <v>500</v>
       </c>
       <c r="D53">
-        <v>22</v>
+        <v>232</v>
       </c>
       <c r="E53">
-        <v>66</v>
+        <v>721</v>
       </c>
       <c r="F53">
-        <v>-128</v>
+        <v>-1295</v>
       </c>
       <c r="G53">
         <f t="shared" si="0"/>
-        <v>-0.82051282051282048</v>
+        <v>-0.80384854127870886</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
@@ -6394,23 +6394,23 @@
         <v>861</v>
       </c>
       <c r="B54">
-        <v>14</v>
+        <v>157</v>
       </c>
       <c r="C54">
-        <v>32</v>
+        <v>406</v>
       </c>
       <c r="D54">
-        <v>18</v>
+        <v>214</v>
       </c>
       <c r="E54">
-        <v>76</v>
+        <v>691</v>
       </c>
       <c r="F54">
-        <v>-112</v>
+        <v>-1154</v>
       </c>
       <c r="G54">
         <f t="shared" si="0"/>
-        <v>-0.8</v>
+        <v>-0.78610354223433243</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
@@ -6418,23 +6418,23 @@
         <v>881</v>
       </c>
       <c r="B55">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="C55">
-        <v>35</v>
+        <v>439</v>
       </c>
       <c r="D55">
-        <v>23</v>
+        <v>232</v>
       </c>
       <c r="E55">
-        <v>63</v>
+        <v>711</v>
       </c>
       <c r="F55">
-        <v>-113</v>
+        <v>-1262</v>
       </c>
       <c r="G55">
         <f t="shared" si="0"/>
-        <v>-0.87596899224806202</v>
+        <v>-0.84021304926764317</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -6442,23 +6442,23 @@
         <v>901</v>
       </c>
       <c r="B56">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="C56">
-        <v>46</v>
+        <v>395</v>
       </c>
       <c r="D56">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="E56">
-        <v>76</v>
+        <v>682</v>
       </c>
       <c r="F56">
-        <v>-142</v>
+        <v>-1158</v>
       </c>
       <c r="G56">
         <f t="shared" si="0"/>
-        <v>-0.93421052631578949</v>
+        <v>-0.84773060029282576</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
@@ -6466,23 +6466,23 @@
         <v>921</v>
       </c>
       <c r="B57">
-        <v>9</v>
+        <v>101</v>
       </c>
       <c r="C57">
-        <v>32</v>
+        <v>344</v>
       </c>
       <c r="D57">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="E57">
-        <v>65</v>
+        <v>611</v>
       </c>
       <c r="F57">
-        <v>-100</v>
+        <v>-1026</v>
       </c>
       <c r="G57">
         <f t="shared" si="0"/>
-        <v>-0.84745762711864403</v>
+        <v>-0.83550488599348538</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
@@ -6490,23 +6490,23 @@
         <v>941</v>
       </c>
       <c r="B58">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C58">
-        <v>33</v>
+        <v>315</v>
       </c>
       <c r="D58">
-        <v>16</v>
+        <v>183</v>
       </c>
       <c r="E58">
-        <v>57</v>
+        <v>642</v>
       </c>
       <c r="F58">
-        <v>-94</v>
+        <v>-1073</v>
       </c>
       <c r="G58">
         <f t="shared" si="0"/>
-        <v>-0.79661016949152541</v>
+        <v>-0.88898094449047227</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -6514,23 +6514,23 @@
         <v>961</v>
       </c>
       <c r="B59">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C59">
-        <v>36</v>
+        <v>301</v>
       </c>
       <c r="D59">
-        <v>22</v>
+        <v>155</v>
       </c>
       <c r="E59">
-        <v>60</v>
+        <v>645</v>
       </c>
       <c r="F59">
-        <v>-113</v>
+        <v>-1034</v>
       </c>
       <c r="G59">
         <f t="shared" si="0"/>
-        <v>-0.91869918699186992</v>
+        <v>-0.88527397260273977</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
@@ -6538,23 +6538,23 @@
         <v>981</v>
       </c>
       <c r="B60">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="C60">
-        <v>35</v>
+        <v>238</v>
       </c>
       <c r="D60">
-        <v>16</v>
+        <v>170</v>
       </c>
       <c r="E60">
-        <v>64</v>
+        <v>683</v>
       </c>
       <c r="F60">
-        <v>-109</v>
+        <v>-1038</v>
       </c>
       <c r="G60">
         <f t="shared" si="0"/>
-        <v>-0.90082644628099173</v>
+        <v>-0.90734265734265729</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -6562,23 +6562,23 @@
         <v>1001</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="C61">
-        <v>22</v>
+        <v>256</v>
       </c>
       <c r="D61">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="E61">
-        <v>57</v>
+        <v>596</v>
       </c>
       <c r="F61">
-        <v>-83</v>
+        <v>-928</v>
       </c>
       <c r="G61">
         <f t="shared" si="0"/>
-        <v>-0.93258426966292129</v>
+        <v>-0.89748549323017413</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
@@ -6586,23 +6586,23 @@
         <v>1021</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="C62">
-        <v>30</v>
+        <v>214</v>
       </c>
       <c r="D62">
-        <v>11</v>
+        <v>139</v>
       </c>
       <c r="E62">
-        <v>61</v>
+        <v>632</v>
       </c>
       <c r="F62">
-        <v>-99</v>
+        <v>-939</v>
       </c>
       <c r="G62">
         <f t="shared" si="0"/>
-        <v>-0.94285714285714284</v>
+        <v>-0.91076624636275461</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -6610,23 +6610,23 @@
         <v>1041</v>
       </c>
       <c r="B63">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C63">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="D63">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="E63">
-        <v>63</v>
+        <v>625</v>
       </c>
       <c r="F63">
-        <v>-85</v>
+        <v>-903</v>
       </c>
       <c r="G63">
         <f t="shared" si="0"/>
-        <v>-0.91397849462365588</v>
+        <v>-0.90936555891238668</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
@@ -6634,23 +6634,23 @@
         <v>1061</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C64">
-        <v>9</v>
+        <v>188</v>
       </c>
       <c r="D64">
-        <v>20</v>
+        <v>122</v>
       </c>
       <c r="E64">
-        <v>56</v>
+        <v>635</v>
       </c>
       <c r="F64">
-        <v>-83</v>
+        <v>-918</v>
       </c>
       <c r="G64">
         <f t="shared" si="0"/>
-        <v>-0.95402298850574707</v>
+        <v>-0.94444444444444442</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
@@ -6658,23 +6658,23 @@
         <v>1081</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="C65">
-        <v>21</v>
+        <v>165</v>
       </c>
       <c r="D65">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="E65">
-        <v>67</v>
+        <v>581</v>
       </c>
       <c r="F65">
-        <v>-96</v>
+        <v>-798</v>
       </c>
       <c r="G65">
         <f t="shared" si="0"/>
-        <v>-0.96</v>
+        <v>-0.92147806004618937</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -6682,23 +6682,23 @@
         <v>1101</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C66">
-        <v>13</v>
+        <v>152</v>
       </c>
       <c r="D66">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="E66">
-        <v>66</v>
+        <v>527</v>
       </c>
       <c r="F66">
-        <v>-88</v>
+        <v>-757</v>
       </c>
       <c r="G66">
         <f t="shared" si="0"/>
-        <v>-0.97777777777777775</v>
+        <v>-0.93572311495673666</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -6706,23 +6706,23 @@
         <v>1121</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C67">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="D67">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="E67">
-        <v>46</v>
+        <v>551</v>
       </c>
       <c r="F67">
-        <v>-77</v>
+        <v>-754</v>
       </c>
       <c r="G67">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-0.93086419753086425</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -6730,23 +6730,23 @@
         <v>1141</v>
       </c>
       <c r="B68">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C68">
-        <v>17</v>
+        <v>126</v>
       </c>
       <c r="D68">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="E68">
-        <v>51</v>
+        <v>572</v>
       </c>
       <c r="F68">
-        <v>-70</v>
+        <v>-762</v>
       </c>
       <c r="G68">
         <f t="shared" si="0"/>
-        <v>-0.94594594594594594</v>
+        <v>-0.94306930693069302</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
@@ -6754,23 +6754,23 @@
         <v>1161</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C69">
-        <v>18</v>
+        <v>128</v>
       </c>
       <c r="D69">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="E69">
-        <v>58</v>
+        <v>570</v>
       </c>
       <c r="F69">
-        <v>-83</v>
+        <v>-754</v>
       </c>
       <c r="G69">
         <f t="shared" si="0"/>
-        <v>-0.97647058823529409</v>
+        <v>-0.94962216624685136</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
@@ -6778,23 +6778,23 @@
         <v>1181</v>
       </c>
       <c r="B70">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C70">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="D70">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="E70">
-        <v>46</v>
+        <v>553</v>
       </c>
       <c r="F70">
-        <v>-61</v>
+        <v>-706</v>
       </c>
       <c r="G70">
         <f t="shared" si="0"/>
-        <v>-0.93846153846153846</v>
+        <v>-0.95405405405405408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>